<commit_message>
merge de todos los archivos
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
+++ b/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Desktop\qualtcom\Organizacional\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Organizacional\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -335,9 +335,6 @@
     <t>Todos los tickets cuentan con una descripcion?</t>
   </si>
   <si>
-    <t>Se asigno un tiempo limite de solucion en los tickets?</t>
-  </si>
-  <si>
     <t>Los tickets tienen un cliente asignado?</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>Los tickets muestran si el cliente cuenta con poliza o no?</t>
+  </si>
+  <si>
+    <t>Se asigno un tiempo de solucion en los tickets?</t>
   </si>
 </sst>
 </file>
@@ -821,6 +821,9 @@
     <xf numFmtId="165" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,9 +857,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1700,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1714,7 +1714,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:1024">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="55" t="s">
         <v>95</v>
       </c>
       <c r="C1" s="49" t="s">
@@ -33583,18 +33583,18 @@
       <c r="AMJ33" s="17"/>
     </row>
     <row r="35" spans="2:1024">
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="54"/>
     </row>
     <row r="36" spans="2:1024">
-      <c r="B36" s="65"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="42" t="s">
         <v>22</v>
       </c>
@@ -33604,7 +33604,7 @@
       <c r="E36" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="53"/>
+      <c r="F36" s="54"/>
     </row>
     <row r="37" spans="2:1024">
       <c r="B37" s="43" t="s">
@@ -33626,7 +33626,7 @@
     </row>
     <row r="39" spans="2:1024">
       <c r="B39" s="43" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C39" s="43"/>
       <c r="D39" s="43"/>
@@ -33635,7 +33635,7 @@
     </row>
     <row r="40" spans="2:1024">
       <c r="B40" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="43"/>
       <c r="D40" s="43"/>
@@ -33644,7 +33644,7 @@
     </row>
     <row r="41" spans="2:1024">
       <c r="B41" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" s="43"/>
       <c r="D41" s="43"/>
@@ -33653,7 +33653,7 @@
     </row>
     <row r="42" spans="2:1024">
       <c r="B42" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -33696,16 +33696,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B2" s="56"/>
-      <c r="C2" s="57" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61" t="s">
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62" t="s">
         <v>57</v>
       </c>
       <c r="H2" s="17"/>
@@ -34727,8 +34727,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="25" t="s">
         <v>58</v>
       </c>
@@ -34738,7 +34738,7 @@
       <c r="F3" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="61"/>
+      <c r="G3" s="62"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -35758,10 +35758,10 @@
       <c r="AMJ3" s="17"/>
     </row>
     <row r="4" spans="2:1024" customFormat="1">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="62"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -39872,10 +39872,10 @@
       <c r="AMJ7" s="17"/>
     </row>
     <row r="8" spans="2:1024" customFormat="1">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -40947,10 +40947,10 @@
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="2:1024" s="31" customFormat="1">
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="62"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -40970,10 +40970,10 @@
     </row>
     <row r="15" spans="2:1024" s="31" customFormat="1"/>
     <row r="16" spans="2:1024" s="31" customFormat="1">
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
     </row>
     <row r="17" spans="4:6" s="31" customFormat="1"/>
     <row r="18" spans="4:6" s="31" customFormat="1">
@@ -40996,10 +40996,10 @@
     <row r="31" spans="4:6" s="31" customFormat="1"/>
     <row r="32" spans="4:6" s="31" customFormat="1"/>
     <row r="33" spans="3:6" s="31" customFormat="1">
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
     </row>
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1">
@@ -41018,10 +41018,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -41035,10 +41035,10 @@
     <row r="52" spans="3:6" s="31" customFormat="1"/>
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1">
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
     </row>
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1">
@@ -41055,10 +41055,10 @@
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
     <row r="65" spans="3:6" s="31" customFormat="1">
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55"/>
-      <c r="F65" s="55"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
     </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
@@ -41074,10 +41074,10 @@
     <row r="73" spans="3:6" s="31" customFormat="1"/>
     <row r="74" spans="3:6" s="31" customFormat="1"/>
     <row r="75" spans="3:6" s="31" customFormat="1">
-      <c r="C75" s="55"/>
-      <c r="D75" s="55"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55"/>
+      <c r="C75" s="56"/>
+      <c r="D75" s="56"/>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56"/>
     </row>
     <row r="76" spans="3:6" s="31" customFormat="1"/>
     <row r="77" spans="3:6" s="31" customFormat="1">
@@ -41106,10 +41106,10 @@
     <row r="96" s="31" customFormat="1"/>
     <row r="97" spans="3:6" s="31" customFormat="1"/>
     <row r="98" spans="3:6" s="31" customFormat="1">
-      <c r="C98" s="55"/>
-      <c r="D98" s="55"/>
-      <c r="E98" s="55"/>
-      <c r="F98" s="55"/>
+      <c r="C98" s="56"/>
+      <c r="D98" s="56"/>
+      <c r="E98" s="56"/>
+      <c r="F98" s="56"/>
     </row>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
     <row r="100" spans="3:6" s="31" customFormat="1">
@@ -41127,10 +41127,10 @@
     <row r="108" spans="3:6" s="31" customFormat="1"/>
     <row r="109" spans="3:6" s="31" customFormat="1"/>
     <row r="110" spans="3:6" s="31" customFormat="1">
-      <c r="C110" s="55"/>
-      <c r="D110" s="55"/>
-      <c r="E110" s="55"/>
-      <c r="F110" s="55"/>
+      <c r="C110" s="56"/>
+      <c r="D110" s="56"/>
+      <c r="E110" s="56"/>
+      <c r="F110" s="56"/>
     </row>
     <row r="111" spans="3:6" s="31" customFormat="1"/>
     <row r="112" spans="3:6" s="31" customFormat="1">
@@ -41152,10 +41152,10 @@
     <row r="124" spans="3:6" s="31" customFormat="1"/>
     <row r="125" spans="3:6" s="31" customFormat="1"/>
     <row r="126" spans="3:6" s="31" customFormat="1">
-      <c r="C126" s="55"/>
-      <c r="D126" s="55"/>
-      <c r="E126" s="55"/>
-      <c r="F126" s="55"/>
+      <c r="C126" s="56"/>
+      <c r="D126" s="56"/>
+      <c r="E126" s="56"/>
+      <c r="F126" s="56"/>
     </row>
     <row r="127" spans="3:6" s="31" customFormat="1"/>
     <row r="128" spans="3:6" s="31" customFormat="1">
@@ -41245,6 +41245,11 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -41256,11 +41261,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -41287,22 +41287,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.45" customHeight="1">
-      <c r="B2" s="56"/>
-      <c r="C2" s="57" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61" t="s">
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="25" t="s">
         <v>58</v>
       </c>
@@ -41312,13 +41312,13 @@
       <c r="F3" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="61"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="62"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -41374,10 +41374,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="62"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
@@ -41447,10 +41447,10 @@
       <c r="G14" s="29"/>
     </row>
     <row r="15" spans="1:7" s="31" customFormat="1">
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="62"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
@@ -41508,10 +41508,10 @@
     <row r="21" spans="2:7" s="31" customFormat="1"/>
     <row r="22" spans="2:7" s="31" customFormat="1"/>
     <row r="23" spans="2:7" s="31" customFormat="1">
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
     </row>
     <row r="24" spans="2:7" s="31" customFormat="1"/>
     <row r="25" spans="2:7" s="31" customFormat="1">
@@ -41530,10 +41530,10 @@
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1"/>
     <row r="36" spans="3:6" s="31" customFormat="1">
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
     </row>
     <row r="37" spans="3:6" s="31" customFormat="1"/>
     <row r="38" spans="3:6" s="31" customFormat="1">
@@ -41547,10 +41547,10 @@
     <row r="42" spans="3:6" s="31" customFormat="1"/>
     <row r="43" spans="3:6" s="31" customFormat="1"/>
     <row r="44" spans="3:6" s="31" customFormat="1">
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
     </row>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
@@ -41567,10 +41567,10 @@
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1"/>
     <row r="55" spans="3:6" s="31" customFormat="1">
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
     </row>
     <row r="56" spans="3:6" s="31" customFormat="1"/>
     <row r="57" spans="3:6" s="31" customFormat="1">
@@ -41586,10 +41586,10 @@
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
     <row r="65" spans="3:6" s="31" customFormat="1">
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55"/>
-      <c r="F65" s="55"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
     </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
@@ -41618,10 +41618,10 @@
     <row r="86" spans="3:6" s="31" customFormat="1"/>
     <row r="87" spans="3:6" s="31" customFormat="1"/>
     <row r="88" spans="3:6" s="31" customFormat="1">
-      <c r="C88" s="55"/>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="55"/>
+      <c r="C88" s="56"/>
+      <c r="D88" s="56"/>
+      <c r="E88" s="56"/>
+      <c r="F88" s="56"/>
     </row>
     <row r="89" spans="3:6" s="31" customFormat="1"/>
     <row r="90" spans="3:6" s="31" customFormat="1">
@@ -41639,10 +41639,10 @@
     <row r="98" spans="3:6" s="31" customFormat="1"/>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
     <row r="100" spans="3:6" s="31" customFormat="1">
-      <c r="C100" s="55"/>
-      <c r="D100" s="55"/>
-      <c r="E100" s="55"/>
-      <c r="F100" s="55"/>
+      <c r="C100" s="56"/>
+      <c r="D100" s="56"/>
+      <c r="E100" s="56"/>
+      <c r="F100" s="56"/>
     </row>
     <row r="101" spans="3:6" s="31" customFormat="1"/>
     <row r="102" spans="3:6" s="31" customFormat="1">
@@ -41664,10 +41664,10 @@
     <row r="114" spans="3:6" s="31" customFormat="1"/>
     <row r="115" spans="3:6" s="31" customFormat="1"/>
     <row r="116" spans="3:6" s="31" customFormat="1">
-      <c r="C116" s="55"/>
-      <c r="D116" s="55"/>
-      <c r="E116" s="55"/>
-      <c r="F116" s="55"/>
+      <c r="C116" s="56"/>
+      <c r="D116" s="56"/>
+      <c r="E116" s="56"/>
+      <c r="F116" s="56"/>
     </row>
     <row r="117" spans="3:6" s="31" customFormat="1"/>
     <row r="118" spans="3:6" s="31" customFormat="1">
@@ -41770,12 +41770,6 @@
     <row r="211" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="C88:F88"/>
     <mergeCell ref="C100:F100"/>
     <mergeCell ref="C116:F116"/>
@@ -41785,6 +41779,12 @@
     <mergeCell ref="C44:F44"/>
     <mergeCell ref="C55:F55"/>
     <mergeCell ref="C65:F65"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -41814,24 +41814,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">

</xml_diff>

<commit_message>
Check list de procesos PTL
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
+++ b/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\qtp\qualtcom\Organizacional\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Organizacional\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>¿El ticket tiene asignada una fecha de compromiso?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -834,10 +837,10 @@
     <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,6 +862,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -885,12 +894,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1553,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ19"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1570,7 +1573,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1">
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="47" t="s">
         <v>79</v>
       </c>
       <c r="D1" s="49" t="s">
@@ -1581,7 +1584,7 @@
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="C2" s="67"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="20" t="s">
         <v>22</v>
       </c>
@@ -1682,7 +1685,7 @@
       <c r="G10" s="23"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="47" t="s">
         <v>86</v>
       </c>
       <c r="D12" s="49" t="s">
@@ -1693,7 +1696,7 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="C13" s="67"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="20" t="s">
         <v>22</v>
       </c>
@@ -1759,6 +1762,11 @@
       <c r="F19" s="22"/>
       <c r="G19" s="23"/>
     </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:C2"/>
@@ -1801,7 +1809,7 @@
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="2:1024">
-      <c r="B2" s="48"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="20" t="s">
         <v>22</v>
       </c>
@@ -15163,7 +15171,7 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="2:1024" customFormat="1">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="57" t="s">
         <v>88</v>
       </c>
       <c r="C16" s="49" t="s">
@@ -16192,7 +16200,7 @@
       <c r="AMJ16" s="17"/>
     </row>
     <row r="17" spans="2:1024" customFormat="1">
-      <c r="B17" s="48"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
@@ -25437,7 +25445,7 @@
       <c r="AMJ25" s="17"/>
     </row>
     <row r="26" spans="2:1024" customFormat="1">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="57" t="s">
         <v>89</v>
       </c>
       <c r="C26" s="49" t="s">
@@ -26466,7 +26474,7 @@
       <c r="AMJ26" s="17"/>
     </row>
     <row r="27" spans="2:1024" customFormat="1" ht="18" customHeight="1">
-      <c r="B27" s="48"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="20" t="s">
         <v>22</v>
       </c>
@@ -32746,16 +32754,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62" t="s">
+      <c r="E2" s="62"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64" t="s">
         <v>53</v>
       </c>
       <c r="H2" s="17"/>
@@ -33777,8 +33785,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="25" t="s">
         <v>54</v>
       </c>
@@ -33788,7 +33796,7 @@
       <c r="F3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="62"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -34808,10 +34816,10 @@
       <c r="AMJ3" s="17"/>
     </row>
     <row r="4" spans="2:1024" customFormat="1">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="63"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -38922,10 +38930,10 @@
       <c r="AMJ7" s="17"/>
     </row>
     <row r="8" spans="2:1024" customFormat="1">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="63"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -39997,10 +40005,10 @@
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="2:1024" s="31" customFormat="1">
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="63"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -40020,10 +40028,10 @@
     </row>
     <row r="15" spans="2:1024" s="31" customFormat="1"/>
     <row r="16" spans="2:1024" s="31" customFormat="1">
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
     </row>
     <row r="17" spans="4:6" s="31" customFormat="1"/>
     <row r="18" spans="4:6" s="31" customFormat="1">
@@ -40046,10 +40054,10 @@
     <row r="31" spans="4:6" s="31" customFormat="1"/>
     <row r="32" spans="4:6" s="31" customFormat="1"/>
     <row r="33" spans="3:6" s="31" customFormat="1">
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
     </row>
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1">
@@ -40068,10 +40076,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40085,10 +40093,10 @@
     <row r="52" spans="3:6" s="31" customFormat="1"/>
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1">
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
     </row>
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1">
@@ -40105,10 +40113,10 @@
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
     <row r="65" spans="3:6" s="31" customFormat="1">
-      <c r="C65" s="56"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58"/>
     </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
@@ -40124,10 +40132,10 @@
     <row r="73" spans="3:6" s="31" customFormat="1"/>
     <row r="74" spans="3:6" s="31" customFormat="1"/>
     <row r="75" spans="3:6" s="31" customFormat="1">
-      <c r="C75" s="56"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="56"/>
-      <c r="F75" s="56"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="58"/>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58"/>
     </row>
     <row r="76" spans="3:6" s="31" customFormat="1"/>
     <row r="77" spans="3:6" s="31" customFormat="1">
@@ -40156,10 +40164,10 @@
     <row r="96" s="31" customFormat="1"/>
     <row r="97" spans="3:6" s="31" customFormat="1"/>
     <row r="98" spans="3:6" s="31" customFormat="1">
-      <c r="C98" s="56"/>
-      <c r="D98" s="56"/>
-      <c r="E98" s="56"/>
-      <c r="F98" s="56"/>
+      <c r="C98" s="58"/>
+      <c r="D98" s="58"/>
+      <c r="E98" s="58"/>
+      <c r="F98" s="58"/>
     </row>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
     <row r="100" spans="3:6" s="31" customFormat="1">
@@ -40177,10 +40185,10 @@
     <row r="108" spans="3:6" s="31" customFormat="1"/>
     <row r="109" spans="3:6" s="31" customFormat="1"/>
     <row r="110" spans="3:6" s="31" customFormat="1">
-      <c r="C110" s="56"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="56"/>
-      <c r="F110" s="56"/>
+      <c r="C110" s="58"/>
+      <c r="D110" s="58"/>
+      <c r="E110" s="58"/>
+      <c r="F110" s="58"/>
     </row>
     <row r="111" spans="3:6" s="31" customFormat="1"/>
     <row r="112" spans="3:6" s="31" customFormat="1">
@@ -40202,10 +40210,10 @@
     <row r="124" spans="3:6" s="31" customFormat="1"/>
     <row r="125" spans="3:6" s="31" customFormat="1"/>
     <row r="126" spans="3:6" s="31" customFormat="1">
-      <c r="C126" s="56"/>
-      <c r="D126" s="56"/>
-      <c r="E126" s="56"/>
-      <c r="F126" s="56"/>
+      <c r="C126" s="58"/>
+      <c r="D126" s="58"/>
+      <c r="E126" s="58"/>
+      <c r="F126" s="58"/>
     </row>
     <row r="127" spans="3:6" s="31" customFormat="1"/>
     <row r="128" spans="3:6" s="31" customFormat="1">
@@ -40295,11 +40303,6 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -40311,6 +40314,11 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40337,22 +40345,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.45" customHeight="1">
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62" t="s">
+      <c r="E2" s="62"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="25" t="s">
         <v>54</v>
       </c>
@@ -40362,13 +40370,13 @@
       <c r="F3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="62"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="63"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -40424,10 +40432,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
@@ -40523,10 +40531,10 @@
       <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" s="31" customFormat="1">
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="63"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
@@ -40584,10 +40592,10 @@
     <row r="23" spans="2:7" s="31" customFormat="1"/>
     <row r="24" spans="2:7" s="31" customFormat="1"/>
     <row r="25" spans="2:7" s="31" customFormat="1">
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
     </row>
     <row r="26" spans="2:7" s="31" customFormat="1"/>
     <row r="27" spans="2:7" s="31" customFormat="1">
@@ -40606,10 +40614,10 @@
     <row r="36" spans="3:6" s="31" customFormat="1"/>
     <row r="37" spans="3:6" s="31" customFormat="1"/>
     <row r="38" spans="3:6" s="31" customFormat="1">
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
     </row>
     <row r="39" spans="3:6" s="31" customFormat="1"/>
     <row r="40" spans="3:6" s="31" customFormat="1">
@@ -40623,10 +40631,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40643,10 +40651,10 @@
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1"/>
     <row r="57" spans="3:6" s="31" customFormat="1">
-      <c r="C57" s="56"/>
-      <c r="D57" s="56"/>
-      <c r="E57" s="56"/>
-      <c r="F57" s="56"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="58"/>
     </row>
     <row r="58" spans="3:6" s="31" customFormat="1"/>
     <row r="59" spans="3:6" s="31" customFormat="1">
@@ -40662,10 +40670,10 @@
     <row r="65" spans="3:6" s="31" customFormat="1"/>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="58"/>
+      <c r="E67" s="58"/>
+      <c r="F67" s="58"/>
     </row>
     <row r="68" spans="3:6" s="31" customFormat="1"/>
     <row r="69" spans="3:6" s="31" customFormat="1">
@@ -40694,10 +40702,10 @@
     <row r="88" spans="3:6" s="31" customFormat="1"/>
     <row r="89" spans="3:6" s="31" customFormat="1"/>
     <row r="90" spans="3:6" s="31" customFormat="1">
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="56"/>
-      <c r="F90" s="56"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="58"/>
+      <c r="E90" s="58"/>
+      <c r="F90" s="58"/>
     </row>
     <row r="91" spans="3:6" s="31" customFormat="1"/>
     <row r="92" spans="3:6" s="31" customFormat="1">
@@ -40715,10 +40723,10 @@
     <row r="100" spans="3:6" s="31" customFormat="1"/>
     <row r="101" spans="3:6" s="31" customFormat="1"/>
     <row r="102" spans="3:6" s="31" customFormat="1">
-      <c r="C102" s="56"/>
-      <c r="D102" s="56"/>
-      <c r="E102" s="56"/>
-      <c r="F102" s="56"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="58"/>
+      <c r="F102" s="58"/>
     </row>
     <row r="103" spans="3:6" s="31" customFormat="1"/>
     <row r="104" spans="3:6" s="31" customFormat="1">
@@ -40740,10 +40748,10 @@
     <row r="116" spans="3:6" s="31" customFormat="1"/>
     <row r="117" spans="3:6" s="31" customFormat="1"/>
     <row r="118" spans="3:6" s="31" customFormat="1">
-      <c r="C118" s="56"/>
-      <c r="D118" s="56"/>
-      <c r="E118" s="56"/>
-      <c r="F118" s="56"/>
+      <c r="C118" s="58"/>
+      <c r="D118" s="58"/>
+      <c r="E118" s="58"/>
+      <c r="F118" s="58"/>
     </row>
     <row r="119" spans="3:6" s="31" customFormat="1"/>
     <row r="120" spans="3:6" s="31" customFormat="1">
@@ -40846,6 +40854,12 @@
     <row r="213" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="C90:F90"/>
     <mergeCell ref="C102:F102"/>
     <mergeCell ref="C118:F118"/>
@@ -40855,12 +40869,6 @@
     <mergeCell ref="C46:F46"/>
     <mergeCell ref="C57:F57"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40890,24 +40898,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">

</xml_diff>

<commit_message>
Actualizacion PTL Checklist Procesos
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
+++ b/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Organizacional\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\qtp\qualtcom\Organizacional\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="1"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -32,25 +32,13 @@
     <t>Nombre del Proyecto</t>
   </si>
   <si>
-    <t>&lt;Nombre del Proyecto&gt;</t>
-  </si>
-  <si>
     <t>Nombre del Responsable del Componente a Evaluar</t>
-  </si>
-  <si>
-    <t>&lt;Persona a ser evaluada&gt;</t>
   </si>
   <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>&lt;Fecha&gt;</t>
-  </si>
-  <si>
     <t>Elaborado por</t>
-  </si>
-  <si>
-    <t>&lt;Aseguramiento de la calidad&gt;</t>
   </si>
   <si>
     <t>Auditoría de Procesos</t>
@@ -302,19 +290,7 @@
     <t xml:space="preserve">Ticket de servicio </t>
   </si>
   <si>
-    <t>Todos los tickets cuentan con una descripcion?</t>
-  </si>
-  <si>
-    <t>Los tickets tienen un cliente asignado?</t>
-  </si>
-  <si>
-    <t>Los tickets cuentan con una fecha de creacion?</t>
-  </si>
-  <si>
     <t>Los tickets muestran si el cliente cuenta con poliza o no?</t>
-  </si>
-  <si>
-    <t>Se asigno un tiempo de solucion en los tickets?</t>
   </si>
   <si>
     <t>¿Se registro el ticket en Mantis?</t>
@@ -335,9 +311,6 @@
     <t>¿Se generó el plan de calidad?</t>
   </si>
   <si>
-    <t>¿Se generó el plan de medición?</t>
-  </si>
-  <si>
     <t>¿Se generó el plan de configuración?</t>
   </si>
   <si>
@@ -350,9 +323,6 @@
     <t>¿Se asignó un responsable por ticket?</t>
   </si>
   <si>
-    <t>¿Se resolvió el ticket en el tiempo especificado?</t>
-  </si>
-  <si>
     <t>¿Se cerró el ticket en la fecha especificada?</t>
   </si>
   <si>
@@ -363,6 +333,57 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>¿Se generó el plan de métricas?</t>
+  </si>
+  <si>
+    <t>¿Los tickets tienen un cliente asignado?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets cuentan con una descripcion?</t>
+  </si>
+  <si>
+    <t>¿Se asignó un tiempo de solucion en los tickets?</t>
+  </si>
+  <si>
+    <t>¿Se notificó al responsable del ticket?</t>
+  </si>
+  <si>
+    <t>¿Se resolvió el ticket?</t>
+  </si>
+  <si>
+    <t>VIA</t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayra Tejeda </t>
+  </si>
+  <si>
+    <t>Junio 19, 2015</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> En estimación de costo por servicio falta especificar el monto que periodicidad tiene (ejemplo: mensual, anual)</t>
+  </si>
+  <si>
+    <t>Por la fecha de aplicación de este checklist falta incluir el del mes de Junio</t>
+  </si>
+  <si>
+    <t>Falta actualizar el Catálogo de Servicios con el nuevo servicio que se agregó(Mantenimiento de impresoras)</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Junio 25, 2015</t>
+  </si>
+  <si>
+    <t>Fidel Reyna</t>
   </si>
 </sst>
 </file>
@@ -483,7 +504,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +557,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD5DADD"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFE6E6FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -733,7 +766,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -828,8 +861,14 @@
     <xf numFmtId="165" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,6 +934,9 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1214,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1234,84 +1276,84 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
-        <v>2</v>
+      <c r="C5" s="48" t="s">
+        <v>109</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="C6" s="46" t="s">
-        <v>4</v>
+      <c r="C6" s="48" t="s">
+        <v>110</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
-      <c r="C7" s="46" t="s">
-        <v>6</v>
+      <c r="C7" s="48" t="s">
+        <v>112</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
-      <c r="C8" s="46" t="s">
-        <v>8</v>
+      <c r="C8" s="48" t="s">
+        <v>111</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B11" s="44" t="s">
-        <v>9</v>
+      <c r="B11" s="46" t="s">
+        <v>5</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -1334,32 +1376,32 @@
         <v>Ejecución</v>
       </c>
       <c r="C14" s="9">
-        <f>COUNTA(Proceso!D14:D19)</f>
+        <f>COUNTA(Proceso!D14:D17)</f>
         <v>0</v>
       </c>
       <c r="D14" s="10" t="e">
-        <f>COUNTIF((Proceso!D14:D19),"x")/(COUNTIF((Proceso!D14:D19),"x")+COUNTIF((Proceso!E14:E19),"x"))</f>
+        <f>COUNTIF((Proceso!D14:D17),"x")/(COUNTIF((Proceso!D14:D17),"x")+COUNTIF((Proceso!E14:E17),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B16" s="44" t="s">
-        <v>13</v>
+      <c r="B16" s="46" t="s">
+        <v>9</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1">
       <c r="B17" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1">
@@ -1372,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="10" t="e">
-        <f>COUNTIF((Proceso!C3:C18),"x")/(COUNTIF((Proceso!C3:C18),"x")+COUNTIF((Proceso!D3:D18),"x"))</f>
+        <f>COUNTIF((Proceso!C3:C16),"x")/(COUNTIF((Proceso!C3:C16),"x")+COUNTIF((Proceso!D3:D16),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1383,7 +1425,7 @@
       </c>
       <c r="C19" s="9">
         <f>COUNTA(Producto!C18:C24)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D19" s="10" t="e">
         <f>COUNTIF((Proceso!D3:D10),"x")/(COUNTIF((Proceso!D3:D10),"x")+COUNTIF((Proceso!E3:E10),"x"))</f>
@@ -1406,11 +1448,11 @@
     </row>
     <row r="21" spans="2:8" ht="19.5" customHeight="1"/>
     <row r="22" spans="2:8" s="5" customFormat="1" ht="15.75">
-      <c r="B22" s="44" t="s">
-        <v>14</v>
+      <c r="B22" s="46" t="s">
+        <v>10</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="11"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1418,52 +1460,52 @@
     </row>
     <row r="23" spans="2:8" s="5" customFormat="1" ht="12.75" customHeight="1">
       <c r="B23" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B24" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C24" s="9">
         <f>COUNTA(Fisica!D5:D7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
-      <c r="D24" s="10" t="e">
+      <c r="D24" s="10">
         <f>COUNTIF((Fisica!D5:D7),"x")/(COUNTIF((Fisica!D5:D7),"x")+COUNTIF((Fisica!E5:E7),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B25" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C25" s="9">
         <f>COUNTA(Fisica!D9:D12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
-      <c r="D25" s="10" t="e">
+      <c r="D25" s="10">
         <f>COUNTIF((Fisica!D9:D12),"x")/(COUNTIF((Fisica!D9:D12),"x")+COUNTIF((Fisica!E9:E12),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B26" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C26" s="9">
         <f>COUNTA(Fisica!D14:D14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="10" t="e">
-        <f>COUNTIF((Proceso!D18:D18),"x")/(COUNTIF((Proceso!D18:D18),"x")+COUNTIF((Proceso!E18:E18),"x"))</f>
-        <v>#DIV/0!</v>
+        <f>COUNTIF((Proceso!#REF!),"x")/(COUNTIF((Proceso!#REF!),"x")+COUNTIF((Proceso!#REF!),"x"))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="27" spans="2:8" s="5" customFormat="1" ht="12.75">
@@ -1474,63 +1516,63 @@
     </row>
     <row r="28" spans="2:8" s="5" customFormat="1" ht="13.9" customHeight="1"/>
     <row r="29" spans="2:8" s="5" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B29" s="44" t="s">
-        <v>19</v>
+      <c r="B29" s="46" t="s">
+        <v>15</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="14"/>
     </row>
     <row r="30" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B30" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E30" s="15"/>
     </row>
     <row r="31" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B31" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C31" s="9">
         <f>COUNTA(Funcional!D5:D8)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
-      <c r="D31" s="10" t="e">
+      <c r="D31" s="10">
         <f>COUNTIF((Funcional!D5:D8),"x")/(COUNTIF((Funcional!D5:D8),"x")+COUNTIF((Funcional!E5:E8),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="E31" s="15"/>
     </row>
     <row r="32" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B32" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C32" s="9">
         <f>COUNTA(Funcional!D10:D14)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
-      <c r="D32" s="10" t="e">
+      <c r="D32" s="10">
         <f>COUNTIF((Funcional!D10:D14),"x")/(COUNTIF((Funcional!D10:D14),"x")+COUNTIF((Funcional!E10:E14),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:4" s="5" customFormat="1" ht="12.75">
       <c r="B33" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C33" s="9">
         <f>COUNTA(Funcional!D18:D21)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
-      <c r="D33" s="10" t="e">
+      <c r="D33" s="10">
         <f>COUNTIF((Funcional!D18:D21),"x")/(COUNTIF((Funcional!D18:D21),"x")+COUNTIF((Funcional!E18:E21),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="2:4" s="5" customFormat="1" ht="12.75"/>
@@ -1556,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ21"/>
+  <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1573,26 +1615,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1">
-      <c r="C1" s="47" t="s">
-        <v>79</v>
+      <c r="C1" s="49" t="s">
+        <v>75</v>
       </c>
-      <c r="D1" s="49" t="s">
-        <v>52</v>
+      <c r="D1" s="51" t="s">
+        <v>48</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="C2" s="48"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G2" s="19"/>
     </row>
@@ -1600,7 +1642,7 @@
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3" s="40" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -1611,7 +1653,7 @@
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="21" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
@@ -1622,7 +1664,7 @@
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5" s="21" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -1633,7 +1675,7 @@
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="21" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -1644,7 +1686,7 @@
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="21" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -1666,7 +1708,7 @@
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="21" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -1677,7 +1719,7 @@
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -1685,32 +1727,32 @@
       <c r="G10" s="23"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="C12" s="47" t="s">
-        <v>86</v>
+      <c r="C12" s="49" t="s">
+        <v>82</v>
       </c>
-      <c r="D12" s="49" t="s">
-        <v>52</v>
+      <c r="D12" s="51" t="s">
+        <v>48</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="C13" s="48"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7">
       <c r="C14" s="40" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -1718,7 +1760,7 @@
       <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="40" t="s">
         <v>107</v>
       </c>
       <c r="D15" s="22"/>
@@ -1727,7 +1769,7 @@
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="40" t="s">
         <v>108</v>
       </c>
       <c r="D16" s="22"/>
@@ -1737,34 +1779,16 @@
     </row>
     <row r="17" spans="3:7">
       <c r="C17" s="21" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
     </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-    </row>
     <row r="19" spans="3:7">
-      <c r="C19" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
-    </row>
-    <row r="21" spans="3:7">
-      <c r="C21" s="17" t="s">
-        <v>112</v>
+      <c r="C19" s="17" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1782,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ41"/>
+  <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1798,32 +1822,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:1024">
-      <c r="B1" s="55" t="s">
-        <v>87</v>
+      <c r="B1" s="57" t="s">
+        <v>83</v>
       </c>
-      <c r="C1" s="49" t="s">
-        <v>52</v>
+      <c r="C1" s="51" t="s">
+        <v>48</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="2:1024">
-      <c r="B2" s="56"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
       <c r="B3" s="21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -2850,7 +2874,7 @@
     </row>
     <row r="4" spans="2:1024" customFormat="1">
       <c r="B4" s="21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -3877,7 +3901,7 @@
     </row>
     <row r="5" spans="2:1024" customFormat="1">
       <c r="B5" s="21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -4904,7 +4928,7 @@
     </row>
     <row r="6" spans="2:1024" customFormat="1">
       <c r="B6" s="21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -5931,7 +5955,7 @@
     </row>
     <row r="7" spans="2:1024" customFormat="1">
       <c r="B7" s="21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -6958,7 +6982,7 @@
     </row>
     <row r="8" spans="2:1024" customFormat="1">
       <c r="B8" s="21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -7985,7 +8009,7 @@
     </row>
     <row r="9" spans="2:1024" customFormat="1">
       <c r="B9" s="21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -9012,7 +9036,7 @@
     </row>
     <row r="10" spans="2:1024" customFormat="1">
       <c r="B10" s="21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -10039,7 +10063,7 @@
     </row>
     <row r="11" spans="2:1024" customFormat="1">
       <c r="B11" s="21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -11066,7 +11090,7 @@
     </row>
     <row r="12" spans="2:1024" customFormat="1">
       <c r="B12" s="21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -12093,7 +12117,7 @@
     </row>
     <row r="13" spans="2:1024" customFormat="1">
       <c r="B13" s="21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -13120,7 +13144,7 @@
     </row>
     <row r="14" spans="2:1024" customFormat="1">
       <c r="B14" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -15171,14 +15195,14 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="2:1024" customFormat="1">
-      <c r="B16" s="57" t="s">
-        <v>88</v>
+      <c r="B16" s="59" t="s">
+        <v>84</v>
       </c>
-      <c r="C16" s="49" t="s">
-        <v>52</v>
+      <c r="C16" s="51" t="s">
+        <v>48</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="18"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -16200,15 +16224,15 @@
       <c r="AMJ16" s="17"/>
     </row>
     <row r="17" spans="2:1024" customFormat="1">
-      <c r="B17" s="56"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="17"/>
@@ -17232,9 +17256,11 @@
     </row>
     <row r="18" spans="2:1024" customFormat="1">
       <c r="B18" s="21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
@@ -18259,9 +18285,11 @@
     </row>
     <row r="19" spans="2:1024" customFormat="1">
       <c r="B19" s="21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="23"/>
@@ -19286,9 +19314,11 @@
     </row>
     <row r="20" spans="2:1024" customFormat="1">
       <c r="B20" s="21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="23"/>
@@ -20313,9 +20343,11 @@
     </row>
     <row r="21" spans="2:1024" customFormat="1">
       <c r="B21" s="21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="23"/>
@@ -21340,9 +21372,11 @@
     </row>
     <row r="22" spans="2:1024" customFormat="1">
       <c r="B22" s="21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
@@ -22367,9 +22401,11 @@
     </row>
     <row r="23" spans="2:1024" customFormat="1">
       <c r="B23" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
@@ -23394,9 +23430,11 @@
     </row>
     <row r="24" spans="2:1024" customFormat="1">
       <c r="B24" s="21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
@@ -25445,14 +25483,14 @@
       <c r="AMJ25" s="17"/>
     </row>
     <row r="26" spans="2:1024" customFormat="1">
-      <c r="B26" s="57" t="s">
-        <v>89</v>
+      <c r="B26" s="59" t="s">
+        <v>85</v>
       </c>
-      <c r="C26" s="49" t="s">
-        <v>52</v>
+      <c r="C26" s="51" t="s">
+        <v>48</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="51"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
       <c r="F26" s="18"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -26474,15 +26512,15 @@
       <c r="AMJ26" s="17"/>
     </row>
     <row r="27" spans="2:1024" customFormat="1" ht="18" customHeight="1">
-      <c r="B27" s="56"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="17"/>
@@ -27506,7 +27544,7 @@
     </row>
     <row r="28" spans="2:1024" customFormat="1">
       <c r="B28" s="16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -28533,7 +28571,7 @@
     </row>
     <row r="29" spans="2:1024" customFormat="1">
       <c r="B29" s="24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -29560,7 +29598,7 @@
     </row>
     <row r="30" spans="2:1024" customFormat="1">
       <c r="B30" s="24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -30587,7 +30625,7 @@
     </row>
     <row r="31" spans="2:1024" customFormat="1">
       <c r="B31" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -31614,7 +31652,7 @@
     </row>
     <row r="32" spans="2:1024" customFormat="1">
       <c r="B32" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -32642,7 +32680,7 @@
     <row r="33" spans="1:6">
       <c r="A33"/>
       <c r="B33" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -32650,73 +32688,91 @@
       <c r="F33" s="16"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="52" t="s">
-        <v>91</v>
+      <c r="B35" s="54" t="s">
+        <v>87</v>
       </c>
-      <c r="C35" s="53" t="s">
-        <v>52</v>
+      <c r="C35" s="55" t="s">
+        <v>48</v>
       </c>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="54"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="56"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="B36" s="52"/>
-      <c r="C36" s="42" t="s">
-        <v>22</v>
+      <c r="B36" s="54"/>
+      <c r="C36" s="43" t="s">
+        <v>18</v>
       </c>
-      <c r="D36" s="42" t="s">
-        <v>23</v>
+      <c r="D36" s="43" t="s">
+        <v>19</v>
       </c>
-      <c r="E36" s="42" t="s">
-        <v>24</v>
+      <c r="E36" s="43" t="s">
+        <v>20</v>
       </c>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="B37" s="43" t="s">
-        <v>92</v>
+      <c r="B37" s="44" t="s">
+        <v>105</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="43" t="s">
-        <v>96</v>
+      <c r="B38" s="44" t="s">
+        <v>106</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="43" t="s">
-        <v>94</v>
+      <c r="B39" s="44" t="s">
+        <v>104</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="43" t="s">
-        <v>93</v>
+      <c r="B40" s="45" t="s">
+        <v>98</v>
       </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="43" t="s">
-        <v>95</v>
+      <c r="B41" s="45" t="s">
+        <v>101</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -32740,8 +32796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMJ208"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32754,17 +32810,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
-        <v>51</v>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>47</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>52</v>
+      <c r="D2" s="63" t="s">
+        <v>48</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64" t="s">
-        <v>53</v>
+      <c r="E2" s="64"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66" t="s">
+        <v>49</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -33785,18 +33841,18 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -34816,10 +34872,10 @@
       <c r="AMJ3" s="17"/>
     </row>
     <row r="4" spans="2:1024" customFormat="1">
-      <c r="B4" s="65" t="s">
-        <v>16</v>
+      <c r="B4" s="67" t="s">
+        <v>12</v>
       </c>
-      <c r="C4" s="65"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -35847,9 +35903,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="29"/>
@@ -36876,9 +36934,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="29"/>
@@ -37905,9 +37965,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="29"/>
@@ -38930,10 +38992,10 @@
       <c r="AMJ7" s="17"/>
     </row>
     <row r="8" spans="2:1024" customFormat="1">
-      <c r="B8" s="65" t="s">
-        <v>17</v>
+      <c r="B8" s="67" t="s">
+        <v>13</v>
       </c>
-      <c r="C8" s="65"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -39961,9 +40023,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
       <c r="G9" s="29"/>
@@ -39973,9 +40037,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="29"/>
@@ -39985,9 +40051,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="29"/>
@@ -39997,18 +40065,20 @@
         <v>7</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="2:1024" s="31" customFormat="1">
-      <c r="B13" s="65" t="s">
-        <v>18</v>
+      <c r="B13" s="67" t="s">
+        <v>14</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -40019,19 +40089,21 @@
         <v>8</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="29"/>
     </row>
     <row r="15" spans="2:1024" s="31" customFormat="1"/>
     <row r="16" spans="2:1024" s="31" customFormat="1">
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="4:6" s="31" customFormat="1"/>
     <row r="18" spans="4:6" s="31" customFormat="1">
@@ -40054,10 +40126,10 @@
     <row r="31" spans="4:6" s="31" customFormat="1"/>
     <row r="32" spans="4:6" s="31" customFormat="1"/>
     <row r="33" spans="3:6" s="31" customFormat="1">
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
     </row>
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1">
@@ -40076,10 +40148,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40093,10 +40165,10 @@
     <row r="52" spans="3:6" s="31" customFormat="1"/>
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1">
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
     </row>
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1">
@@ -40113,10 +40185,10 @@
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
     <row r="65" spans="3:6" s="31" customFormat="1">
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="60"/>
     </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
@@ -40132,10 +40204,10 @@
     <row r="73" spans="3:6" s="31" customFormat="1"/>
     <row r="74" spans="3:6" s="31" customFormat="1"/>
     <row r="75" spans="3:6" s="31" customFormat="1">
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
+      <c r="C75" s="60"/>
+      <c r="D75" s="60"/>
+      <c r="E75" s="60"/>
+      <c r="F75" s="60"/>
     </row>
     <row r="76" spans="3:6" s="31" customFormat="1"/>
     <row r="77" spans="3:6" s="31" customFormat="1">
@@ -40164,10 +40236,10 @@
     <row r="96" s="31" customFormat="1"/>
     <row r="97" spans="3:6" s="31" customFormat="1"/>
     <row r="98" spans="3:6" s="31" customFormat="1">
-      <c r="C98" s="58"/>
-      <c r="D98" s="58"/>
-      <c r="E98" s="58"/>
-      <c r="F98" s="58"/>
+      <c r="C98" s="60"/>
+      <c r="D98" s="60"/>
+      <c r="E98" s="60"/>
+      <c r="F98" s="60"/>
     </row>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
     <row r="100" spans="3:6" s="31" customFormat="1">
@@ -40185,10 +40257,10 @@
     <row r="108" spans="3:6" s="31" customFormat="1"/>
     <row r="109" spans="3:6" s="31" customFormat="1"/>
     <row r="110" spans="3:6" s="31" customFormat="1">
-      <c r="C110" s="58"/>
-      <c r="D110" s="58"/>
-      <c r="E110" s="58"/>
-      <c r="F110" s="58"/>
+      <c r="C110" s="60"/>
+      <c r="D110" s="60"/>
+      <c r="E110" s="60"/>
+      <c r="F110" s="60"/>
     </row>
     <row r="111" spans="3:6" s="31" customFormat="1"/>
     <row r="112" spans="3:6" s="31" customFormat="1">
@@ -40210,10 +40282,10 @@
     <row r="124" spans="3:6" s="31" customFormat="1"/>
     <row r="125" spans="3:6" s="31" customFormat="1"/>
     <row r="126" spans="3:6" s="31" customFormat="1">
-      <c r="C126" s="58"/>
-      <c r="D126" s="58"/>
-      <c r="E126" s="58"/>
-      <c r="F126" s="58"/>
+      <c r="C126" s="60"/>
+      <c r="D126" s="60"/>
+      <c r="E126" s="60"/>
+      <c r="F126" s="60"/>
     </row>
     <row r="127" spans="3:6" s="31" customFormat="1"/>
     <row r="128" spans="3:6" s="31" customFormat="1">
@@ -40303,6 +40375,11 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -40314,11 +40391,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40331,7 +40403,7 @@
   <dimension ref="A2:AMJ213"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40345,38 +40417,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.45" customHeight="1">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
-        <v>51</v>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>47</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>52</v>
+      <c r="D2" s="63" t="s">
+        <v>48</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64" t="s">
-        <v>53</v>
+      <c r="E2" s="64"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="65" t="s">
-        <v>20</v>
+      <c r="B4" s="67" t="s">
+        <v>16</v>
       </c>
-      <c r="C4" s="65"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -40387,9 +40459,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="36"/>
@@ -40399,9 +40473,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="29"/>
@@ -40411,9 +40487,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="36"/>
@@ -40423,44 +40501,52 @@
         <v>4</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="65" t="s">
-        <v>21</v>
+      <c r="B9" s="67" t="s">
+        <v>17</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:7" s="31" customFormat="1">
+    <row r="10" spans="1:7" s="31" customFormat="1" ht="38.25">
       <c r="B10" s="28">
         <v>1</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="29"/>
+      <c r="G10" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" spans="1:7" s="31" customFormat="1">
       <c r="B11" s="28">
         <v>2</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="29"/>
@@ -40471,9 +40557,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="29"/>
@@ -40484,9 +40572,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
       <c r="G13" s="29"/>
@@ -40497,25 +40587,33 @@
         <v>5</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
-      <c r="G14" s="29"/>
+      <c r="G14" s="29" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="25.5">
       <c r="A15"/>
       <c r="B15" s="28">
         <v>6</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
-      <c r="G15" s="29"/>
+      <c r="G15" s="29" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="38.25">
       <c r="A16"/>
@@ -40523,18 +40621,22 @@
         <v>7</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
-      <c r="D16" s="30"/>
+      <c r="D16" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="29"/>
+      <c r="G16" s="29" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="17" spans="2:7" s="31" customFormat="1">
-      <c r="B17" s="65" t="s">
-        <v>18</v>
+      <c r="B17" s="67" t="s">
+        <v>14</v>
       </c>
-      <c r="C17" s="65"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
@@ -40545,9 +40647,11 @@
         <v>1</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="36"/>
@@ -40557,9 +40661,11 @@
         <v>2</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="29"/>
@@ -40569,10 +40675,12 @@
         <v>3</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="E20" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="F20" s="30"/>
       <c r="G20" s="29"/>
     </row>
@@ -40581,10 +40689,12 @@
         <v>4</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="E21" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="F21" s="30"/>
       <c r="G21" s="29"/>
     </row>
@@ -40592,10 +40702,10 @@
     <row r="23" spans="2:7" s="31" customFormat="1"/>
     <row r="24" spans="2:7" s="31" customFormat="1"/>
     <row r="25" spans="2:7" s="31" customFormat="1">
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
     </row>
     <row r="26" spans="2:7" s="31" customFormat="1"/>
     <row r="27" spans="2:7" s="31" customFormat="1">
@@ -40614,10 +40724,10 @@
     <row r="36" spans="3:6" s="31" customFormat="1"/>
     <row r="37" spans="3:6" s="31" customFormat="1"/>
     <row r="38" spans="3:6" s="31" customFormat="1">
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
     </row>
     <row r="39" spans="3:6" s="31" customFormat="1"/>
     <row r="40" spans="3:6" s="31" customFormat="1">
@@ -40631,10 +40741,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40651,10 +40761,10 @@
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1"/>
     <row r="57" spans="3:6" s="31" customFormat="1">
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
     </row>
     <row r="58" spans="3:6" s="31" customFormat="1"/>
     <row r="59" spans="3:6" s="31" customFormat="1">
@@ -40670,10 +40780,10 @@
     <row r="65" spans="3:6" s="31" customFormat="1"/>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="58"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="60"/>
+      <c r="F67" s="60"/>
     </row>
     <row r="68" spans="3:6" s="31" customFormat="1"/>
     <row r="69" spans="3:6" s="31" customFormat="1">
@@ -40702,10 +40812,10 @@
     <row r="88" spans="3:6" s="31" customFormat="1"/>
     <row r="89" spans="3:6" s="31" customFormat="1"/>
     <row r="90" spans="3:6" s="31" customFormat="1">
-      <c r="C90" s="58"/>
-      <c r="D90" s="58"/>
-      <c r="E90" s="58"/>
-      <c r="F90" s="58"/>
+      <c r="C90" s="60"/>
+      <c r="D90" s="60"/>
+      <c r="E90" s="60"/>
+      <c r="F90" s="60"/>
     </row>
     <row r="91" spans="3:6" s="31" customFormat="1"/>
     <row r="92" spans="3:6" s="31" customFormat="1">
@@ -40723,10 +40833,10 @@
     <row r="100" spans="3:6" s="31" customFormat="1"/>
     <row r="101" spans="3:6" s="31" customFormat="1"/>
     <row r="102" spans="3:6" s="31" customFormat="1">
-      <c r="C102" s="58"/>
-      <c r="D102" s="58"/>
-      <c r="E102" s="58"/>
-      <c r="F102" s="58"/>
+      <c r="C102" s="60"/>
+      <c r="D102" s="60"/>
+      <c r="E102" s="60"/>
+      <c r="F102" s="60"/>
     </row>
     <row r="103" spans="3:6" s="31" customFormat="1"/>
     <row r="104" spans="3:6" s="31" customFormat="1">
@@ -40748,10 +40858,10 @@
     <row r="116" spans="3:6" s="31" customFormat="1"/>
     <row r="117" spans="3:6" s="31" customFormat="1"/>
     <row r="118" spans="3:6" s="31" customFormat="1">
-      <c r="C118" s="58"/>
-      <c r="D118" s="58"/>
-      <c r="E118" s="58"/>
-      <c r="F118" s="58"/>
+      <c r="C118" s="60"/>
+      <c r="D118" s="60"/>
+      <c r="E118" s="60"/>
+      <c r="F118" s="60"/>
     </row>
     <row r="119" spans="3:6" s="31" customFormat="1"/>
     <row r="120" spans="3:6" s="31" customFormat="1">
@@ -40854,12 +40964,6 @@
     <row r="213" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="C90:F90"/>
     <mergeCell ref="C102:F102"/>
     <mergeCell ref="C118:F118"/>
@@ -40869,6 +40973,12 @@
     <mergeCell ref="C46:F46"/>
     <mergeCell ref="C57:F57"/>
     <mergeCell ref="C67:F67"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40881,7 +40991,7 @@
   <dimension ref="B3:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40898,55 +41008,65 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B3" s="66" t="s">
-        <v>72</v>
+      <c r="B3" s="68" t="s">
+        <v>68</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="G5" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="41" t="s">
+      <c r="H5" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="41" t="s">
-        <v>77</v>
+    </row>
+    <row r="6" spans="2:8" ht="45">
+      <c r="B6" s="16">
+        <v>1</v>
       </c>
-      <c r="G5" s="41" t="s">
-        <v>78</v>
+      <c r="C6" s="70" t="s">
+        <v>116</v>
       </c>
-      <c r="H5" s="41" t="s">
-        <v>80</v>
+      <c r="D6" s="16" t="s">
+        <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>118</v>
+      </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8">

</xml_diff>

<commit_message>
Actualización Plantilla  Checklist Procesos
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
+++ b/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -363,27 +363,6 @@
   </si>
   <si>
     <t>Junio 19, 2015</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> En estimación de costo por servicio falta especificar el monto que periodicidad tiene (ejemplo: mensual, anual)</t>
-  </si>
-  <si>
-    <t>Por la fecha de aplicación de este checklist falta incluir el del mes de Junio</t>
-  </si>
-  <si>
-    <t>Falta actualizar el Catálogo de Servicios con el nuevo servicio que se agregó(Mantenimiento de impresoras)</t>
-  </si>
-  <si>
-    <t>En proceso</t>
-  </si>
-  <si>
-    <t>Junio 25, 2015</t>
-  </si>
-  <si>
-    <t>Fidel Reyna</t>
   </si>
 </sst>
 </file>
@@ -869,6 +848,9 @@
     <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,9 +916,6 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1256,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -1276,73 +1255,73 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
@@ -1386,11 +1365,11 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1">
@@ -1425,7 +1404,7 @@
       </c>
       <c r="C19" s="9">
         <f>COUNTA(Producto!C18:C24)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D19" s="10" t="e">
         <f>COUNTIF((Proceso!D3:D10),"x")/(COUNTIF((Proceso!D3:D10),"x")+COUNTIF((Proceso!E3:E10),"x"))</f>
@@ -1448,11 +1427,11 @@
     </row>
     <row r="21" spans="2:8" ht="19.5" customHeight="1"/>
     <row r="22" spans="2:8" s="5" customFormat="1" ht="15.75">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="11"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1475,11 +1454,11 @@
       </c>
       <c r="C24" s="9">
         <f>COUNTA(Fisica!D5:D7)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="10" t="e">
         <f>COUNTIF((Fisica!D5:D7),"x")/(COUNTIF((Fisica!D5:D7),"x")+COUNTIF((Fisica!E5:E7),"x"))</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="2:8" s="5" customFormat="1" ht="12.75">
@@ -1488,11 +1467,11 @@
       </c>
       <c r="C25" s="9">
         <f>COUNTA(Fisica!D9:D12)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="10" t="e">
         <f>COUNTIF((Fisica!D9:D12),"x")/(COUNTIF((Fisica!D9:D12),"x")+COUNTIF((Fisica!E9:E12),"x"))</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="2:8" s="5" customFormat="1" ht="12.75">
@@ -1501,11 +1480,11 @@
       </c>
       <c r="C26" s="9">
         <f>COUNTA(Fisica!D14:D14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="10" t="e">
-        <f>COUNTIF((Proceso!#REF!),"x")/(COUNTIF((Proceso!#REF!),"x")+COUNTIF((Proceso!#REF!),"x"))</f>
-        <v>#REF!</v>
+        <f>COUNTIF((Fisica!D14),"x")/(COUNTIF((Fisica!D14),"x")+COUNTIF((Fisica!E14),"x"))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="2:8" s="5" customFormat="1" ht="12.75">
@@ -1516,11 +1495,11 @@
     </row>
     <row r="28" spans="2:8" s="5" customFormat="1" ht="13.9" customHeight="1"/>
     <row r="29" spans="2:8" s="5" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
       <c r="E29" s="14"/>
     </row>
     <row r="30" spans="2:8" s="5" customFormat="1" ht="12.75">
@@ -1541,11 +1520,11 @@
       </c>
       <c r="C31" s="9">
         <f>COUNTA(Funcional!D5:D8)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="10" t="e">
         <f>COUNTIF((Funcional!D5:D8),"x")/(COUNTIF((Funcional!D5:D8),"x")+COUNTIF((Funcional!E5:E8),"x"))</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E31" s="15"/>
     </row>
@@ -1555,11 +1534,11 @@
       </c>
       <c r="C32" s="9">
         <f>COUNTA(Funcional!D10:D14)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="10" t="e">
         <f>COUNTIF((Funcional!D10:D14),"x")/(COUNTIF((Funcional!D10:D14),"x")+COUNTIF((Funcional!E10:E14),"x"))</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="2:4" s="5" customFormat="1" ht="12.75">
@@ -1568,11 +1547,11 @@
       </c>
       <c r="C33" s="9">
         <f>COUNTA(Funcional!D18:D21)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="10" t="e">
         <f>COUNTIF((Funcional!D18:D21),"x")/(COUNTIF((Funcional!D18:D21),"x")+COUNTIF((Funcional!E18:E21),"x"))</f>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="2:4" s="5" customFormat="1" ht="12.75"/>
@@ -1615,18 +1594,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1">
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="54"/>
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="C2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="20" t="s">
         <v>18</v>
       </c>
@@ -1727,18 +1706,18 @@
       <c r="G10" s="23"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="C13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="20" t="s">
         <v>18</v>
       </c>
@@ -1808,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1822,18 +1801,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:1024">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="2:1024">
-      <c r="B2" s="58"/>
+      <c r="B2" s="59"/>
       <c r="C2" s="20" t="s">
         <v>18</v>
       </c>
@@ -15195,14 +15174,14 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="2:1024" customFormat="1">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="18"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -16224,7 +16203,7 @@
       <c r="AMJ16" s="17"/>
     </row>
     <row r="17" spans="2:1024" customFormat="1">
-      <c r="B17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="20" t="s">
         <v>18</v>
       </c>
@@ -17258,9 +17237,7 @@
       <c r="B18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
@@ -18287,9 +18264,7 @@
       <c r="B19" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="23"/>
@@ -19316,9 +19291,7 @@
       <c r="B20" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="23"/>
@@ -20345,9 +20318,7 @@
       <c r="B21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C21" s="22"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="23"/>
@@ -21374,9 +21345,7 @@
       <c r="B22" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
@@ -22403,9 +22372,7 @@
       <c r="B23" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
@@ -23432,9 +23399,7 @@
       <c r="B24" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
@@ -25483,14 +25448,14 @@
       <c r="AMJ25" s="17"/>
     </row>
     <row r="26" spans="2:1024" customFormat="1">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="18"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -26512,7 +26477,7 @@
       <c r="AMJ26" s="17"/>
     </row>
     <row r="27" spans="2:1024" customFormat="1" ht="18" customHeight="1">
-      <c r="B27" s="58"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="20" t="s">
         <v>18</v>
       </c>
@@ -32688,18 +32653,18 @@
       <c r="F33" s="16"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="57"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="B36" s="54"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="43" t="s">
         <v>18</v>
       </c>
@@ -32709,7 +32674,7 @@
       <c r="E36" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="56"/>
+      <c r="F36" s="57"/>
     </row>
     <row r="37" spans="1:6">
       <c r="B37" s="44" t="s">
@@ -32797,7 +32762,7 @@
   <dimension ref="A2:AMJ208"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D5" sqref="D5:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32810,16 +32775,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B2" s="61"/>
-      <c r="C2" s="62" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="17"/>
@@ -33841,8 +33806,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
-      <c r="B3" s="61"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="25" t="s">
         <v>50</v>
       </c>
@@ -33852,7 +33817,7 @@
       <c r="F3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="67"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -34872,10 +34837,10 @@
       <c r="AMJ3" s="17"/>
     </row>
     <row r="4" spans="2:1024" customFormat="1">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="67"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -35905,9 +35870,7 @@
       <c r="C5" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="29"/>
@@ -36936,9 +36899,7 @@
       <c r="C6" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D6" s="30"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="29"/>
@@ -37967,9 +37928,7 @@
       <c r="C7" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="29"/>
@@ -38992,10 +38951,10 @@
       <c r="AMJ7" s="17"/>
     </row>
     <row r="8" spans="2:1024" customFormat="1">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -40025,9 +39984,7 @@
       <c r="C9" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D9" s="30"/>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
       <c r="G9" s="29"/>
@@ -40039,9 +39996,7 @@
       <c r="C10" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D10" s="30"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="29"/>
@@ -40053,9 +40008,7 @@
       <c r="C11" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D11" s="30"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="29"/>
@@ -40067,18 +40020,16 @@
       <c r="C12" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D12" s="30"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="2:1024" s="31" customFormat="1">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="68"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -40091,19 +40042,17 @@
       <c r="C14" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="29"/>
     </row>
     <row r="15" spans="2:1024" s="31" customFormat="1"/>
     <row r="16" spans="2:1024" s="31" customFormat="1">
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
     </row>
     <row r="17" spans="4:6" s="31" customFormat="1"/>
     <row r="18" spans="4:6" s="31" customFormat="1">
@@ -40126,10 +40075,10 @@
     <row r="31" spans="4:6" s="31" customFormat="1"/>
     <row r="32" spans="4:6" s="31" customFormat="1"/>
     <row r="33" spans="3:6" s="31" customFormat="1">
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
     </row>
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1">
@@ -40148,10 +40097,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40165,10 +40114,10 @@
     <row r="52" spans="3:6" s="31" customFormat="1"/>
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1">
-      <c r="C54" s="60"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="60"/>
-      <c r="F54" s="60"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
     </row>
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1">
@@ -40185,10 +40134,10 @@
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
     <row r="65" spans="3:6" s="31" customFormat="1">
-      <c r="C65" s="60"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="61"/>
+      <c r="F65" s="61"/>
     </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
@@ -40204,10 +40153,10 @@
     <row r="73" spans="3:6" s="31" customFormat="1"/>
     <row r="74" spans="3:6" s="31" customFormat="1"/>
     <row r="75" spans="3:6" s="31" customFormat="1">
-      <c r="C75" s="60"/>
-      <c r="D75" s="60"/>
-      <c r="E75" s="60"/>
-      <c r="F75" s="60"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
     </row>
     <row r="76" spans="3:6" s="31" customFormat="1"/>
     <row r="77" spans="3:6" s="31" customFormat="1">
@@ -40236,10 +40185,10 @@
     <row r="96" s="31" customFormat="1"/>
     <row r="97" spans="3:6" s="31" customFormat="1"/>
     <row r="98" spans="3:6" s="31" customFormat="1">
-      <c r="C98" s="60"/>
-      <c r="D98" s="60"/>
-      <c r="E98" s="60"/>
-      <c r="F98" s="60"/>
+      <c r="C98" s="61"/>
+      <c r="D98" s="61"/>
+      <c r="E98" s="61"/>
+      <c r="F98" s="61"/>
     </row>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
     <row r="100" spans="3:6" s="31" customFormat="1">
@@ -40257,10 +40206,10 @@
     <row r="108" spans="3:6" s="31" customFormat="1"/>
     <row r="109" spans="3:6" s="31" customFormat="1"/>
     <row r="110" spans="3:6" s="31" customFormat="1">
-      <c r="C110" s="60"/>
-      <c r="D110" s="60"/>
-      <c r="E110" s="60"/>
-      <c r="F110" s="60"/>
+      <c r="C110" s="61"/>
+      <c r="D110" s="61"/>
+      <c r="E110" s="61"/>
+      <c r="F110" s="61"/>
     </row>
     <row r="111" spans="3:6" s="31" customFormat="1"/>
     <row r="112" spans="3:6" s="31" customFormat="1">
@@ -40282,10 +40231,10 @@
     <row r="124" spans="3:6" s="31" customFormat="1"/>
     <row r="125" spans="3:6" s="31" customFormat="1"/>
     <row r="126" spans="3:6" s="31" customFormat="1">
-      <c r="C126" s="60"/>
-      <c r="D126" s="60"/>
-      <c r="E126" s="60"/>
-      <c r="F126" s="60"/>
+      <c r="C126" s="61"/>
+      <c r="D126" s="61"/>
+      <c r="E126" s="61"/>
+      <c r="F126" s="61"/>
     </row>
     <row r="127" spans="3:6" s="31" customFormat="1"/>
     <row r="128" spans="3:6" s="31" customFormat="1">
@@ -40403,7 +40352,7 @@
   <dimension ref="A2:AMJ213"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G10" sqref="G10:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40417,22 +40366,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.45" customHeight="1">
-      <c r="B2" s="61"/>
-      <c r="C2" s="62" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="61"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="25" t="s">
         <v>50</v>
       </c>
@@ -40442,13 +40391,13 @@
       <c r="F3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="67"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -40461,9 +40410,7 @@
       <c r="C5" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="36"/>
@@ -40475,9 +40422,7 @@
       <c r="C6" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D6" s="30"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="29"/>
@@ -40489,9 +40434,7 @@
       <c r="C7" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="36"/>
@@ -40503,39 +40446,33 @@
       <c r="C8" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="67"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:7" s="31" customFormat="1" ht="38.25">
+    <row r="10" spans="1:7" s="31" customFormat="1">
       <c r="B10" s="28">
         <v>1</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D10" s="30"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="29" t="s">
-        <v>114</v>
-      </c>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:7" s="31" customFormat="1">
       <c r="B11" s="28">
@@ -40544,9 +40481,7 @@
       <c r="C11" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D11" s="30"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="29"/>
@@ -40559,9 +40494,7 @@
       <c r="C12" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D12" s="30"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="29"/>
@@ -40574,9 +40507,7 @@
       <c r="C13" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D13" s="30"/>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
       <c r="G13" s="29"/>
@@ -40589,16 +40520,12 @@
       <c r="C14" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
-      <c r="G14" s="29" t="s">
-        <v>115</v>
-      </c>
+      <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="1:7" ht="25.5">
+    <row r="15" spans="1:7">
       <c r="A15"/>
       <c r="B15" s="28">
         <v>6</v>
@@ -40606,14 +40533,10 @@
       <c r="C15" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
-      <c r="G15" s="29" t="s">
-        <v>115</v>
-      </c>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="38.25">
       <c r="A16"/>
@@ -40623,20 +40546,16 @@
       <c r="C16" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="29" t="s">
-        <v>115</v>
-      </c>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" s="31" customFormat="1">
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="67"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
@@ -40649,9 +40568,7 @@
       <c r="C18" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="36"/>
@@ -40663,9 +40580,7 @@
       <c r="C19" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="29"/>
@@ -40678,9 +40593,7 @@
         <v>66</v>
       </c>
       <c r="D20" s="30"/>
-      <c r="E20" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="29"/>
     </row>
@@ -40692,9 +40605,7 @@
         <v>67</v>
       </c>
       <c r="D21" s="30"/>
-      <c r="E21" s="30" t="s">
-        <v>113</v>
-      </c>
+      <c r="E21" s="30"/>
       <c r="F21" s="30"/>
       <c r="G21" s="29"/>
     </row>
@@ -40702,10 +40613,10 @@
     <row r="23" spans="2:7" s="31" customFormat="1"/>
     <row r="24" spans="2:7" s="31" customFormat="1"/>
     <row r="25" spans="2:7" s="31" customFormat="1">
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
     </row>
     <row r="26" spans="2:7" s="31" customFormat="1"/>
     <row r="27" spans="2:7" s="31" customFormat="1">
@@ -40724,10 +40635,10 @@
     <row r="36" spans="3:6" s="31" customFormat="1"/>
     <row r="37" spans="3:6" s="31" customFormat="1"/>
     <row r="38" spans="3:6" s="31" customFormat="1">
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
     </row>
     <row r="39" spans="3:6" s="31" customFormat="1"/>
     <row r="40" spans="3:6" s="31" customFormat="1">
@@ -40741,10 +40652,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40761,10 +40672,10 @@
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1"/>
     <row r="57" spans="3:6" s="31" customFormat="1">
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="60"/>
-      <c r="F57" s="60"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61"/>
     </row>
     <row r="58" spans="3:6" s="31" customFormat="1"/>
     <row r="59" spans="3:6" s="31" customFormat="1">
@@ -40780,10 +40691,10 @@
     <row r="65" spans="3:6" s="31" customFormat="1"/>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
-      <c r="C67" s="60"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
-      <c r="F67" s="60"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="61"/>
+      <c r="F67" s="61"/>
     </row>
     <row r="68" spans="3:6" s="31" customFormat="1"/>
     <row r="69" spans="3:6" s="31" customFormat="1">
@@ -40812,10 +40723,10 @@
     <row r="88" spans="3:6" s="31" customFormat="1"/>
     <row r="89" spans="3:6" s="31" customFormat="1"/>
     <row r="90" spans="3:6" s="31" customFormat="1">
-      <c r="C90" s="60"/>
-      <c r="D90" s="60"/>
-      <c r="E90" s="60"/>
-      <c r="F90" s="60"/>
+      <c r="C90" s="61"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="61"/>
     </row>
     <row r="91" spans="3:6" s="31" customFormat="1"/>
     <row r="92" spans="3:6" s="31" customFormat="1">
@@ -40833,10 +40744,10 @@
     <row r="100" spans="3:6" s="31" customFormat="1"/>
     <row r="101" spans="3:6" s="31" customFormat="1"/>
     <row r="102" spans="3:6" s="31" customFormat="1">
-      <c r="C102" s="60"/>
-      <c r="D102" s="60"/>
-      <c r="E102" s="60"/>
-      <c r="F102" s="60"/>
+      <c r="C102" s="61"/>
+      <c r="D102" s="61"/>
+      <c r="E102" s="61"/>
+      <c r="F102" s="61"/>
     </row>
     <row r="103" spans="3:6" s="31" customFormat="1"/>
     <row r="104" spans="3:6" s="31" customFormat="1">
@@ -40858,10 +40769,10 @@
     <row r="116" spans="3:6" s="31" customFormat="1"/>
     <row r="117" spans="3:6" s="31" customFormat="1"/>
     <row r="118" spans="3:6" s="31" customFormat="1">
-      <c r="C118" s="60"/>
-      <c r="D118" s="60"/>
-      <c r="E118" s="60"/>
-      <c r="F118" s="60"/>
+      <c r="C118" s="61"/>
+      <c r="D118" s="61"/>
+      <c r="E118" s="61"/>
+      <c r="F118" s="61"/>
     </row>
     <row r="119" spans="3:6" s="31" customFormat="1"/>
     <row r="120" spans="3:6" s="31" customFormat="1">
@@ -40991,7 +40902,7 @@
   <dimension ref="B3:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -41008,24 +40919,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
     </row>
     <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">
@@ -41050,24 +40961,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="45">
-      <c r="B6" s="16">
-        <v>1</v>
-      </c>
-      <c r="C6" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>118</v>
-      </c>
+    <row r="6" spans="2:8">
+      <c r="B6" s="16"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="16"/>

</xml_diff>

<commit_message>
Actualización Plantilla Checklist de Procesos
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
+++ b/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
@@ -353,16 +353,16 @@
     <t>¿Se resolvió el ticket?</t>
   </si>
   <si>
-    <t>VIA</t>
+    <t>&lt;Nombre del Proyecto&gt;</t>
   </si>
   <si>
-    <t>Jovanny Zepeda</t>
+    <t>&lt;Persona a ser evaluada&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Mayra Tejeda </t>
+    <t>&lt;Fecha&gt;</t>
   </si>
   <si>
-    <t>Junio 19, 2015</t>
+    <t>&lt;Aseguramiento de la calidad&gt;</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -855,9 +855,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -916,6 +913,15 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1235,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1274,45 +1280,45 @@
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>112</v>
+      <c r="C7" s="70" t="s">
+        <v>111</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>111</v>
+      <c r="C8" s="70" t="s">
+        <v>112</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="72"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
@@ -1594,18 +1600,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1">
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="54"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="C2" s="51"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="20" t="s">
         <v>18</v>
       </c>
@@ -1706,18 +1712,18 @@
       <c r="G10" s="23"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="54"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="C13" s="51"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="20" t="s">
         <v>18</v>
       </c>
@@ -1801,18 +1807,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:1024">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="2:1024">
-      <c r="B2" s="59"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="20" t="s">
         <v>18</v>
       </c>
@@ -15174,14 +15180,14 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="2:1024" customFormat="1">
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="54"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="18"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -16203,7 +16209,7 @@
       <c r="AMJ16" s="17"/>
     </row>
     <row r="17" spans="2:1024" customFormat="1">
-      <c r="B17" s="59"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="20" t="s">
         <v>18</v>
       </c>
@@ -25448,14 +25454,14 @@
       <c r="AMJ25" s="17"/>
     </row>
     <row r="26" spans="2:1024" customFormat="1">
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="54"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
       <c r="F26" s="18"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -26477,7 +26483,7 @@
       <c r="AMJ26" s="17"/>
     </row>
     <row r="27" spans="2:1024" customFormat="1" ht="18" customHeight="1">
-      <c r="B27" s="59"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="20" t="s">
         <v>18</v>
       </c>
@@ -32653,18 +32659,18 @@
       <c r="F33" s="16"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="57"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="56"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="B36" s="55"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="43" t="s">
         <v>18</v>
       </c>
@@ -32674,7 +32680,7 @@
       <c r="E36" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="57"/>
+      <c r="F36" s="56"/>
     </row>
     <row r="37" spans="1:6">
       <c r="B37" s="44" t="s">
@@ -32775,16 +32781,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
-      <c r="B2" s="62"/>
-      <c r="C2" s="63" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="17"/>
@@ -33806,8 +33812,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="25" t="s">
         <v>50</v>
       </c>
@@ -33817,7 +33823,7 @@
       <c r="F3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="67"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -34837,10 +34843,10 @@
       <c r="AMJ3" s="17"/>
     </row>
     <row r="4" spans="2:1024" customFormat="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -38951,10 +38957,10 @@
       <c r="AMJ7" s="17"/>
     </row>
     <row r="8" spans="2:1024" customFormat="1">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -40026,10 +40032,10 @@
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="2:1024" s="31" customFormat="1">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="68"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -40049,10 +40055,10 @@
     </row>
     <row r="15" spans="2:1024" s="31" customFormat="1"/>
     <row r="16" spans="2:1024" s="31" customFormat="1">
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="4:6" s="31" customFormat="1"/>
     <row r="18" spans="4:6" s="31" customFormat="1">
@@ -40075,10 +40081,10 @@
     <row r="31" spans="4:6" s="31" customFormat="1"/>
     <row r="32" spans="4:6" s="31" customFormat="1"/>
     <row r="33" spans="3:6" s="31" customFormat="1">
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
     </row>
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1">
@@ -40097,10 +40103,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40114,10 +40120,10 @@
     <row r="52" spans="3:6" s="31" customFormat="1"/>
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1">
-      <c r="C54" s="61"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
     </row>
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1">
@@ -40134,10 +40140,10 @@
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
     <row r="65" spans="3:6" s="31" customFormat="1">
-      <c r="C65" s="61"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="60"/>
     </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
@@ -40153,10 +40159,10 @@
     <row r="73" spans="3:6" s="31" customFormat="1"/>
     <row r="74" spans="3:6" s="31" customFormat="1"/>
     <row r="75" spans="3:6" s="31" customFormat="1">
-      <c r="C75" s="61"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="61"/>
+      <c r="C75" s="60"/>
+      <c r="D75" s="60"/>
+      <c r="E75" s="60"/>
+      <c r="F75" s="60"/>
     </row>
     <row r="76" spans="3:6" s="31" customFormat="1"/>
     <row r="77" spans="3:6" s="31" customFormat="1">
@@ -40185,10 +40191,10 @@
     <row r="96" s="31" customFormat="1"/>
     <row r="97" spans="3:6" s="31" customFormat="1"/>
     <row r="98" spans="3:6" s="31" customFormat="1">
-      <c r="C98" s="61"/>
-      <c r="D98" s="61"/>
-      <c r="E98" s="61"/>
-      <c r="F98" s="61"/>
+      <c r="C98" s="60"/>
+      <c r="D98" s="60"/>
+      <c r="E98" s="60"/>
+      <c r="F98" s="60"/>
     </row>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
     <row r="100" spans="3:6" s="31" customFormat="1">
@@ -40206,10 +40212,10 @@
     <row r="108" spans="3:6" s="31" customFormat="1"/>
     <row r="109" spans="3:6" s="31" customFormat="1"/>
     <row r="110" spans="3:6" s="31" customFormat="1">
-      <c r="C110" s="61"/>
-      <c r="D110" s="61"/>
-      <c r="E110" s="61"/>
-      <c r="F110" s="61"/>
+      <c r="C110" s="60"/>
+      <c r="D110" s="60"/>
+      <c r="E110" s="60"/>
+      <c r="F110" s="60"/>
     </row>
     <row r="111" spans="3:6" s="31" customFormat="1"/>
     <row r="112" spans="3:6" s="31" customFormat="1">
@@ -40231,10 +40237,10 @@
     <row r="124" spans="3:6" s="31" customFormat="1"/>
     <row r="125" spans="3:6" s="31" customFormat="1"/>
     <row r="126" spans="3:6" s="31" customFormat="1">
-      <c r="C126" s="61"/>
-      <c r="D126" s="61"/>
-      <c r="E126" s="61"/>
-      <c r="F126" s="61"/>
+      <c r="C126" s="60"/>
+      <c r="D126" s="60"/>
+      <c r="E126" s="60"/>
+      <c r="F126" s="60"/>
     </row>
     <row r="127" spans="3:6" s="31" customFormat="1"/>
     <row r="128" spans="3:6" s="31" customFormat="1">
@@ -40324,11 +40330,6 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -40340,6 +40341,11 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40366,22 +40372,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.45" customHeight="1">
-      <c r="B2" s="62"/>
-      <c r="C2" s="63" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="25" t="s">
         <v>50</v>
       </c>
@@ -40391,13 +40397,13 @@
       <c r="F3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="67"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -40453,10 +40459,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="68"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
@@ -40552,10 +40558,10 @@
       <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" s="31" customFormat="1">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
@@ -40613,10 +40619,10 @@
     <row r="23" spans="2:7" s="31" customFormat="1"/>
     <row r="24" spans="2:7" s="31" customFormat="1"/>
     <row r="25" spans="2:7" s="31" customFormat="1">
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
     </row>
     <row r="26" spans="2:7" s="31" customFormat="1"/>
     <row r="27" spans="2:7" s="31" customFormat="1">
@@ -40635,10 +40641,10 @@
     <row r="36" spans="3:6" s="31" customFormat="1"/>
     <row r="37" spans="3:6" s="31" customFormat="1"/>
     <row r="38" spans="3:6" s="31" customFormat="1">
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
     </row>
     <row r="39" spans="3:6" s="31" customFormat="1"/>
     <row r="40" spans="3:6" s="31" customFormat="1">
@@ -40652,10 +40658,10 @@
     <row r="44" spans="3:6" s="31" customFormat="1"/>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
     <row r="48" spans="3:6" s="31" customFormat="1">
@@ -40672,10 +40678,10 @@
     <row r="55" spans="3:6" s="31" customFormat="1"/>
     <row r="56" spans="3:6" s="31" customFormat="1"/>
     <row r="57" spans="3:6" s="31" customFormat="1">
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
     </row>
     <row r="58" spans="3:6" s="31" customFormat="1"/>
     <row r="59" spans="3:6" s="31" customFormat="1">
@@ -40691,10 +40697,10 @@
     <row r="65" spans="3:6" s="31" customFormat="1"/>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
-      <c r="C67" s="61"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="61"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="60"/>
+      <c r="F67" s="60"/>
     </row>
     <row r="68" spans="3:6" s="31" customFormat="1"/>
     <row r="69" spans="3:6" s="31" customFormat="1">
@@ -40723,10 +40729,10 @@
     <row r="88" spans="3:6" s="31" customFormat="1"/>
     <row r="89" spans="3:6" s="31" customFormat="1"/>
     <row r="90" spans="3:6" s="31" customFormat="1">
-      <c r="C90" s="61"/>
-      <c r="D90" s="61"/>
-      <c r="E90" s="61"/>
-      <c r="F90" s="61"/>
+      <c r="C90" s="60"/>
+      <c r="D90" s="60"/>
+      <c r="E90" s="60"/>
+      <c r="F90" s="60"/>
     </row>
     <row r="91" spans="3:6" s="31" customFormat="1"/>
     <row r="92" spans="3:6" s="31" customFormat="1">
@@ -40744,10 +40750,10 @@
     <row r="100" spans="3:6" s="31" customFormat="1"/>
     <row r="101" spans="3:6" s="31" customFormat="1"/>
     <row r="102" spans="3:6" s="31" customFormat="1">
-      <c r="C102" s="61"/>
-      <c r="D102" s="61"/>
-      <c r="E102" s="61"/>
-      <c r="F102" s="61"/>
+      <c r="C102" s="60"/>
+      <c r="D102" s="60"/>
+      <c r="E102" s="60"/>
+      <c r="F102" s="60"/>
     </row>
     <row r="103" spans="3:6" s="31" customFormat="1"/>
     <row r="104" spans="3:6" s="31" customFormat="1">
@@ -40769,10 +40775,10 @@
     <row r="116" spans="3:6" s="31" customFormat="1"/>
     <row r="117" spans="3:6" s="31" customFormat="1"/>
     <row r="118" spans="3:6" s="31" customFormat="1">
-      <c r="C118" s="61"/>
-      <c r="D118" s="61"/>
-      <c r="E118" s="61"/>
-      <c r="F118" s="61"/>
+      <c r="C118" s="60"/>
+      <c r="D118" s="60"/>
+      <c r="E118" s="60"/>
+      <c r="F118" s="60"/>
     </row>
     <row r="119" spans="3:6" s="31" customFormat="1"/>
     <row r="120" spans="3:6" s="31" customFormat="1">
@@ -40875,6 +40881,12 @@
     <row r="213" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="C90:F90"/>
     <mergeCell ref="C102:F102"/>
     <mergeCell ref="C118:F118"/>
@@ -40884,12 +40896,6 @@
     <mergeCell ref="C46:F46"/>
     <mergeCell ref="C57:F57"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40919,24 +40925,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">

</xml_diff>